<commit_message>
1. delete all card 2. test add Credit card --- visa, master, AMEX, Discovery determine site payment gateway 3. test add credit card to Freedom pay 4. test add credit card to exact
</commit_message>
<xml_diff>
--- a/register.xlsx
+++ b/register.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larry.li/SourceTree/jtt/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
@@ -76,12 +76,16 @@
   </si>
   <si>
     <t>PWD</t>
+  </si>
+  <si>
+    <t>W.A.901150038@mailsac.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -427,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5FAFD5-CFE1-A34A-BEB5-9A8788FE9C4F}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -435,8 +439,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -535,6 +539,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Jtt account setting (pull request #54)"
</commit_message>
<xml_diff>
--- a/register.xlsx
+++ b/register.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larry.li/SourceTree/jtt/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -76,16 +76,12 @@
   </si>
   <si>
     <t>PWD</t>
-  </si>
-  <si>
-    <t>W.A.901150038@mailsac.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -431,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5FAFD5-CFE1-A34A-BEB5-9A8788FE9C4F}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -439,8 +435,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
+    <col min="1" max="1" width="45.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -539,14 +535,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>